<commit_message>
commit adding test case for motor
</commit_message>
<xml_diff>
--- a/ATA_Upload/TestData_ATA.xlsx
+++ b/ATA_Upload/TestData_ATA.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="423">
   <si>
     <t>NO</t>
   </si>
@@ -1483,43 +1483,40 @@
     <t>Electrical issue</t>
   </si>
   <si>
-    <t>TOWING XYZ</t>
-  </si>
-  <si>
-    <t>TAA230</t>
-  </si>
-  <si>
-    <t>TAA231</t>
-  </si>
-  <si>
-    <t>TAA232</t>
-  </si>
-  <si>
-    <t>TAA233</t>
-  </si>
-  <si>
-    <t>TAA234</t>
-  </si>
-  <si>
-    <t>TAA235</t>
-  </si>
-  <si>
-    <t>TAA236</t>
-  </si>
-  <si>
-    <t>TAA237</t>
-  </si>
-  <si>
-    <t>TAA238</t>
-  </si>
-  <si>
-    <t>TAA239</t>
-  </si>
-  <si>
-    <t>TAA240</t>
-  </si>
-  <si>
-    <t>TAA241</t>
+    <t>TAA255</t>
+  </si>
+  <si>
+    <t>TAA256</t>
+  </si>
+  <si>
+    <t>TAA257</t>
+  </si>
+  <si>
+    <t>TAA258</t>
+  </si>
+  <si>
+    <t>TAA259</t>
+  </si>
+  <si>
+    <t>TAA260</t>
+  </si>
+  <si>
+    <t>TAA261</t>
+  </si>
+  <si>
+    <t>TAA262</t>
+  </si>
+  <si>
+    <t>TAA263</t>
+  </si>
+  <si>
+    <t>TAA264</t>
+  </si>
+  <si>
+    <t>TAA265</t>
+  </si>
+  <si>
+    <t>TAA266</t>
   </si>
 </sst>
 </file>
@@ -2595,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="46">
-        <v>123456790120</v>
+        <v>123456790144</v>
       </c>
       <c r="C2" s="46">
         <v>123456788</v>
@@ -2604,7 +2601,7 @@
         <v>123456777</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F2" s="42" t="s">
         <v>409</v>
@@ -2699,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="46">
-        <v>123456790121</v>
+        <v>123456790145</v>
       </c>
       <c r="C3" s="46">
         <v>123456788</v>
@@ -2708,7 +2705,7 @@
         <v>123456777</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F3" s="42" t="s">
         <v>391</v>
@@ -2782,7 +2779,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="46">
-        <v>123456790122</v>
+        <v>123456790146</v>
       </c>
       <c r="C4" s="46">
         <v>123456788</v>
@@ -2791,7 +2788,7 @@
         <v>123456777</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F4" s="42" t="s">
         <v>392</v>
@@ -2865,7 +2862,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="46">
-        <v>123456790123</v>
+        <v>123456790147</v>
       </c>
       <c r="C5" s="46">
         <v>123456788</v>
@@ -2874,7 +2871,7 @@
         <v>123456777</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F5" s="42" t="s">
         <v>393</v>
@@ -2948,7 +2945,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="46">
-        <v>123456790124</v>
+        <v>123456790148</v>
       </c>
       <c r="C6" s="46">
         <v>123456788</v>
@@ -2957,7 +2954,7 @@
         <v>123456777</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F6" s="42" t="s">
         <v>394</v>
@@ -3004,7 +3001,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="46">
-        <v>123456790125</v>
+        <v>123456790149</v>
       </c>
       <c r="C7" s="46">
         <v>123456788</v>
@@ -3013,7 +3010,7 @@
         <v>123456777</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F7" s="42" t="s">
         <v>395</v>
@@ -3060,7 +3057,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="46">
-        <v>123456790126</v>
+        <v>123456790150</v>
       </c>
       <c r="C8" s="46">
         <v>123456788</v>
@@ -3069,7 +3066,7 @@
         <v>123456777</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F8" s="42" t="s">
         <v>396</v>
@@ -3116,7 +3113,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46">
-        <v>123456790127</v>
+        <v>123456790151</v>
       </c>
       <c r="C9" s="46">
         <v>123456788</v>
@@ -3125,7 +3122,7 @@
         <v>123456777</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F9" s="42" t="s">
         <v>397</v>
@@ -3172,7 +3169,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46">
-        <v>123456790128</v>
+        <v>123456790152</v>
       </c>
       <c r="C10" s="46">
         <v>123456788</v>
@@ -3181,7 +3178,7 @@
         <v>123456777</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>398</v>
@@ -3217,7 +3214,7 @@
         <v>282</v>
       </c>
       <c r="Y10" s="42" t="s">
-        <v>411</v>
+        <v>66</v>
       </c>
       <c r="AB10" s="42" t="s">
         <v>16</v>
@@ -3237,7 +3234,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="46">
-        <v>123456790129</v>
+        <v>123456790153</v>
       </c>
       <c r="C11" s="46">
         <v>123456788</v>
@@ -3246,7 +3243,7 @@
         <v>123456777</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F11" s="42" t="s">
         <v>399</v>
@@ -3282,7 +3279,7 @@
         <v>282</v>
       </c>
       <c r="Y11" s="42" t="s">
-        <v>411</v>
+        <v>66</v>
       </c>
       <c r="AB11" s="42" t="s">
         <v>16</v>
@@ -3302,7 +3299,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="46">
-        <v>123456790130</v>
+        <v>123456790154</v>
       </c>
       <c r="C12" s="46">
         <v>123456788</v>
@@ -3311,7 +3308,7 @@
         <v>123456777</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F12" s="42" t="s">
         <v>400</v>
@@ -3347,7 +3344,7 @@
         <v>282</v>
       </c>
       <c r="Y12" s="42" t="s">
-        <v>411</v>
+        <v>66</v>
       </c>
       <c r="AB12" s="42" t="s">
         <v>16</v>
@@ -3367,7 +3364,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="46">
-        <v>123456790131</v>
+        <v>123456790155</v>
       </c>
       <c r="C13" s="46">
         <v>123456788</v>
@@ -3376,7 +3373,7 @@
         <v>123456777</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F13" s="42" t="s">
         <v>401</v>
@@ -3413,7 +3410,7 @@
         <v>282</v>
       </c>
       <c r="Y13" s="42" t="s">
-        <v>411</v>
+        <v>66</v>
       </c>
       <c r="AB13" s="42" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
enhance workshop and tariff module
</commit_message>
<xml_diff>
--- a/ATA_Upload/TestData_ATA.xlsx
+++ b/ATA_Upload/TestData_ATA.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="429">
   <si>
     <t>NO</t>
   </si>
@@ -1483,40 +1483,58 @@
     <t>Electrical issue</t>
   </si>
   <si>
-    <t>TAA255</t>
-  </si>
-  <si>
-    <t>TAA256</t>
-  </si>
-  <si>
-    <t>TAA257</t>
-  </si>
-  <si>
-    <t>TAA258</t>
-  </si>
-  <si>
-    <t>TAA259</t>
-  </si>
-  <si>
-    <t>TAA260</t>
-  </si>
-  <si>
-    <t>TAA261</t>
-  </si>
-  <si>
-    <t>TAA262</t>
-  </si>
-  <si>
-    <t>TAA263</t>
-  </si>
-  <si>
-    <t>TAA264</t>
-  </si>
-  <si>
-    <t>TAA265</t>
-  </si>
-  <si>
-    <t>TAA266</t>
+    <t>case</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>WXM2211</t>
+  </si>
+  <si>
+    <t>Bengkel Setia</t>
+  </si>
+  <si>
+    <t>Fordcon Motor Works Sdn Bhd</t>
+  </si>
+  <si>
+    <t>TAA303</t>
+  </si>
+  <si>
+    <t>TAA304</t>
+  </si>
+  <si>
+    <t>TAA305</t>
+  </si>
+  <si>
+    <t>TAA306</t>
+  </si>
+  <si>
+    <t>TAA307</t>
+  </si>
+  <si>
+    <t>TAA308</t>
+  </si>
+  <si>
+    <t>TAA309</t>
+  </si>
+  <si>
+    <t>TAA310</t>
+  </si>
+  <si>
+    <t>TAA311</t>
+  </si>
+  <si>
+    <t>TAA312</t>
+  </si>
+  <si>
+    <t>TAA313</t>
+  </si>
+  <si>
+    <t>TAA314</t>
   </si>
 </sst>
 </file>
@@ -2439,208 +2457,212 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM18"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="F2" sqref="F2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1" s="49" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="D1" s="49" t="s">
         <v>265</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="E1" s="49" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="F1" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="G1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="H1" s="48" t="s">
         <v>268</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="I1" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="J1" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="K1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="L1" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="M1" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="N1" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="O1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="P1" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="Q1" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="R1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="S1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="T1" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="U1" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="V1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="W1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="X1" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48" t="s">
         <v>276</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="Z1" s="48" t="s">
         <v>277</v>
       </c>
-      <c r="Z1" s="48" t="s">
+      <c r="AA1" s="48" t="s">
         <v>278</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AB1" s="48" t="s">
         <v>279</v>
       </c>
-      <c r="AB1" s="48" t="s">
+      <c r="AC1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="48" t="s">
+      <c r="AD1" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="AD1" s="48" t="s">
+      <c r="AE1" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="AE1" s="48" t="s">
+      <c r="AF1" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="AG1" s="48" t="s">
+      <c r="AH1" s="48" t="s">
         <v>381</v>
       </c>
-      <c r="AH1" s="48" t="s">
+      <c r="AI1" s="48" t="s">
         <v>377</v>
       </c>
-      <c r="AI1" s="48" t="s">
+      <c r="AJ1" s="48" t="s">
         <v>378</v>
       </c>
-      <c r="AJ1" s="48" t="s">
+      <c r="AK1" s="48" t="s">
         <v>379</v>
       </c>
-      <c r="AK1" s="48" t="s">
+      <c r="AL1" s="48" t="s">
         <v>380</v>
       </c>
-      <c r="AL1" s="48" t="s">
+      <c r="AM1" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="AM1" s="48" t="s">
+      <c r="AN1" s="48" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="42">
         <v>1</v>
       </c>
-      <c r="B2" s="46">
-        <v>123456790144</v>
+      <c r="B2" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C2" s="46">
+        <v>123456790181</v>
+      </c>
+      <c r="D2" s="46">
         <v>123456788</v>
       </c>
-      <c r="D2" s="46">
+      <c r="E2" s="46">
         <v>123456777</v>
       </c>
-      <c r="E2" s="42" t="s">
-        <v>411</v>
-      </c>
       <c r="F2" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" s="42" t="s">
         <v>409</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="H2" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="I2" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="J2" s="42" t="s">
         <v>280</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="K2" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="L2" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="N2" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="O2" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="P2" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="P2" s="60" t="s">
+      <c r="Q2" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="Q2" s="42" t="s">
+      <c r="R2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="42" t="s">
+      <c r="S2" s="42" t="s">
         <v>17</v>
-      </c>
-      <c r="S2" s="42" t="s">
-        <v>16</v>
       </c>
       <c r="T2" s="42" t="s">
         <v>16</v>
@@ -2649,102 +2671,105 @@
         <v>16</v>
       </c>
       <c r="V2" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>282</v>
       </c>
-      <c r="Y2" s="42" t="s">
+      <c r="Z2" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="42" t="s">
+      <c r="AC2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>283</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>284</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>285</v>
       </c>
-      <c r="AG2" s="58" t="s">
+      <c r="AH2" s="58" t="s">
         <v>382</v>
       </c>
-      <c r="AH2" s="59">
+      <c r="AI2" s="59">
         <v>1234567898</v>
       </c>
-      <c r="AI2" s="58" t="s">
+      <c r="AJ2" s="58" t="s">
         <v>383</v>
       </c>
-      <c r="AJ2" s="58" t="s">
+      <c r="AK2" s="58" t="s">
         <v>384</v>
       </c>
-      <c r="AK2" s="58">
+      <c r="AL2" s="58">
         <v>84100</v>
       </c>
-      <c r="AL2" s="58" t="s">
+      <c r="AM2" s="58" t="s">
         <v>385</v>
       </c>
-      <c r="AM2" s="58" t="s">
+      <c r="AN2" s="58" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="42">
         <v>2</v>
       </c>
-      <c r="B3" s="46">
-        <v>123456790145</v>
+      <c r="B3" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C3" s="46">
+        <v>123456790182</v>
+      </c>
+      <c r="D3" s="46">
         <v>123456788</v>
       </c>
-      <c r="D3" s="46">
+      <c r="E3" s="46">
         <v>123456777</v>
       </c>
-      <c r="E3" s="42" t="s">
-        <v>412</v>
-      </c>
       <c r="F3" s="42" t="s">
+        <v>418</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>391</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="H3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="42" t="s">
+      <c r="I3" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="J3" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="K3" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="L3" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="N3" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N3" s="42" t="s">
+      <c r="O3" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="P3" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>294</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="R3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="42" t="s">
+      <c r="S3" s="42" t="s">
         <v>16</v>
-      </c>
-      <c r="S3" s="42" t="s">
-        <v>17</v>
       </c>
       <c r="T3" s="42" t="s">
         <v>17</v>
@@ -2753,772 +2778,919 @@
         <v>17</v>
       </c>
       <c r="V3" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>282</v>
       </c>
-      <c r="Y3" s="42" t="s">
+      <c r="Z3" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB3" s="42" t="s">
+      <c r="AC3" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>283</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>284</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="42">
         <v>3</v>
       </c>
-      <c r="B4" s="46">
-        <v>123456790146</v>
+      <c r="B4" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C4" s="46">
+        <v>123456790183</v>
+      </c>
+      <c r="D4" s="46">
         <v>123456788</v>
       </c>
-      <c r="D4" s="46">
+      <c r="E4" s="46">
         <v>123456777</v>
       </c>
-      <c r="E4" s="42" t="s">
-        <v>413</v>
-      </c>
       <c r="F4" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="G4" s="42" t="s">
         <v>392</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="H4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="I4" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="J4" s="42" t="s">
         <v>280</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="K4" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="L4" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="43" t="s">
+      <c r="N4" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N4" s="42" t="s">
+      <c r="O4" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="44" t="s">
+      <c r="P4" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>296</v>
       </c>
-      <c r="Q4" s="42" t="s">
+      <c r="R4" s="42" t="s">
         <v>16</v>
-      </c>
-      <c r="R4" s="42" t="s">
-        <v>17</v>
       </c>
       <c r="S4" s="42" t="s">
         <v>17</v>
       </c>
       <c r="T4" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="42" t="s">
+      <c r="V4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="V4" s="42" t="s">
+      <c r="W4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>282</v>
       </c>
-      <c r="Y4" s="42" t="s">
+      <c r="Z4" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB4" s="42" t="s">
+      <c r="AC4" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>283</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>284</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AH4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="42">
         <v>4</v>
       </c>
-      <c r="B5" s="46">
-        <v>123456790147</v>
+      <c r="B5" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C5" s="46">
+        <v>123456790184</v>
+      </c>
+      <c r="D5" s="46">
         <v>123456788</v>
       </c>
-      <c r="D5" s="46">
+      <c r="E5" s="46">
         <v>123456777</v>
       </c>
-      <c r="E5" s="42" t="s">
-        <v>414</v>
-      </c>
       <c r="F5" s="42" t="s">
+        <v>420</v>
+      </c>
+      <c r="G5" s="42" t="s">
         <v>393</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="H5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="I5" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="J5" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="K5" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="L5" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="43" t="s">
+      <c r="N5" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N5" s="42" t="s">
+      <c r="O5" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="P5" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>410</v>
       </c>
-      <c r="Q5" s="42" t="s">
+      <c r="R5" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="R5" s="42" t="s">
+      <c r="S5" s="42" t="s">
         <v>16</v>
-      </c>
-      <c r="S5" s="42" t="s">
-        <v>17</v>
       </c>
       <c r="T5" s="42" t="s">
         <v>17</v>
       </c>
       <c r="U5" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="42" t="s">
+      <c r="W5" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>282</v>
       </c>
-      <c r="Y5" s="42" t="s">
+      <c r="Z5" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB5" s="42" t="s">
+      <c r="AC5" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>283</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>284</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>5</v>
       </c>
-      <c r="B6" s="46">
-        <v>123456790148</v>
+      <c r="B6" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C6" s="46">
+        <v>123456790185</v>
+      </c>
+      <c r="D6" s="46">
         <v>123456788</v>
       </c>
-      <c r="D6" s="46">
+      <c r="E6" s="46">
         <v>123456777</v>
       </c>
-      <c r="E6" s="42" t="s">
-        <v>415</v>
-      </c>
       <c r="F6" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="G6" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="H6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="I6" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="J6" s="42" t="s">
         <v>280</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="K6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="L6" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="N6" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N6" s="42" t="s">
+      <c r="O6" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="53" t="s">
+      <c r="P6" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="P6" s="54" t="s">
+      <c r="Q6" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>282</v>
       </c>
-      <c r="Y6" s="42" t="s">
+      <c r="Z6" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB6" s="42" t="s">
+      <c r="AC6" s="42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="42">
         <v>6</v>
       </c>
-      <c r="B7" s="46">
-        <v>123456790149</v>
+      <c r="B7" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C7" s="46">
+        <v>123456790186</v>
+      </c>
+      <c r="D7" s="46">
         <v>123456788</v>
       </c>
-      <c r="D7" s="46">
+      <c r="E7" s="46">
         <v>123456777</v>
       </c>
-      <c r="E7" s="42" t="s">
-        <v>416</v>
-      </c>
       <c r="F7" s="42" t="s">
+        <v>422</v>
+      </c>
+      <c r="G7" s="42" t="s">
         <v>395</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="H7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="I7" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="J7" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="K7" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="L7" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="N7" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N7" s="42" t="s">
+      <c r="O7" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="53" t="s">
+      <c r="P7" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="P7" s="54" t="s">
+      <c r="Q7" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>282</v>
       </c>
-      <c r="Y7" s="42" t="s">
+      <c r="Z7" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB7" s="42" t="s">
+      <c r="AC7" s="42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="42">
         <v>7</v>
       </c>
-      <c r="B8" s="46">
-        <v>123456790150</v>
+      <c r="B8" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C8" s="46">
+        <v>123456790187</v>
+      </c>
+      <c r="D8" s="46">
         <v>123456788</v>
       </c>
-      <c r="D8" s="46">
+      <c r="E8" s="46">
         <v>123456777</v>
       </c>
-      <c r="E8" s="42" t="s">
-        <v>417</v>
-      </c>
       <c r="F8" s="42" t="s">
+        <v>423</v>
+      </c>
+      <c r="G8" s="42" t="s">
         <v>396</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="H8" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="I8" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="42" t="s">
+      <c r="J8" s="42" t="s">
         <v>280</v>
       </c>
-      <c r="J8" s="42" t="s">
+      <c r="K8" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="42" t="s">
+      <c r="L8" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="N8" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="O8" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="53" t="s">
+      <c r="P8" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="P8" s="54" t="s">
+      <c r="Q8" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>282</v>
       </c>
-      <c r="Y8" s="42" t="s">
+      <c r="Z8" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB8" s="42" t="s">
+      <c r="AC8" s="42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>8</v>
       </c>
-      <c r="B9" s="46">
-        <v>123456790151</v>
+      <c r="B9" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C9" s="46">
+        <v>123456790188</v>
+      </c>
+      <c r="D9" s="46">
         <v>123456788</v>
       </c>
-      <c r="D9" s="46">
+      <c r="E9" s="46">
         <v>123456777</v>
       </c>
-      <c r="E9" s="42" t="s">
-        <v>418</v>
-      </c>
       <c r="F9" s="42" t="s">
+        <v>424</v>
+      </c>
+      <c r="G9" s="42" t="s">
         <v>397</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="H9" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="I9" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="J9" s="42" t="s">
         <v>405</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="K9" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="42" t="s">
+      <c r="L9" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="N9" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="O9" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="53" t="s">
+      <c r="P9" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="P9" s="54" t="s">
+      <c r="Q9" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>282</v>
       </c>
-      <c r="Y9" s="42" t="s">
+      <c r="Z9" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB9" s="42" t="s">
+      <c r="AC9" s="42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>9</v>
       </c>
-      <c r="B10" s="46">
-        <v>123456790152</v>
+      <c r="B10" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C10" s="46">
+        <v>123456790189</v>
+      </c>
+      <c r="D10" s="46">
         <v>123456788</v>
       </c>
-      <c r="D10" s="46">
+      <c r="E10" s="46">
         <v>123456777</v>
       </c>
-      <c r="E10" s="42" t="s">
-        <v>419</v>
-      </c>
       <c r="F10" s="42" t="s">
+        <v>425</v>
+      </c>
+      <c r="G10" s="42" t="s">
         <v>398</v>
       </c>
-      <c r="G10" s="42" t="s">
+      <c r="H10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="I10" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="J10" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="K10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="42" t="s">
+      <c r="L10" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="N10" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N10" s="42" t="s">
+      <c r="O10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="62" t="s">
+      <c r="P10" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="P10" s="64" t="s">
+      <c r="Q10" s="64" t="s">
         <v>132</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>282</v>
       </c>
-      <c r="Y10" s="42" t="s">
+      <c r="Z10" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB10" s="42" t="s">
+      <c r="AC10" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>283</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>284</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="42">
         <v>10</v>
       </c>
-      <c r="B11" s="46">
-        <v>123456790153</v>
+      <c r="B11" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C11" s="46">
+        <v>123456790190</v>
+      </c>
+      <c r="D11" s="46">
         <v>123456788</v>
       </c>
-      <c r="D11" s="46">
+      <c r="E11" s="46">
         <v>123456777</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>420</v>
-      </c>
       <c r="F11" s="42" t="s">
+        <v>426</v>
+      </c>
+      <c r="G11" s="42" t="s">
         <v>399</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="H11" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="42" t="s">
+      <c r="I11" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="J11" s="42" t="s">
         <v>404</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="K11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="42" t="s">
+      <c r="L11" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="43" t="s">
+      <c r="N11" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N11" s="42" t="s">
+      <c r="O11" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="62" t="s">
+      <c r="P11" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="P11" s="64" t="s">
+      <c r="Q11" s="64" t="s">
         <v>406</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>282</v>
       </c>
-      <c r="Y11" s="42" t="s">
+      <c r="Z11" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB11" s="42" t="s">
+      <c r="AC11" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>283</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>284</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="42">
         <v>11</v>
       </c>
-      <c r="B12" s="46">
-        <v>123456790154</v>
+      <c r="B12" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C12" s="46">
+        <v>123456790191</v>
+      </c>
+      <c r="D12" s="46">
         <v>123456788</v>
       </c>
-      <c r="D12" s="46">
+      <c r="E12" s="46">
         <v>123456777</v>
       </c>
-      <c r="E12" s="42" t="s">
-        <v>421</v>
-      </c>
       <c r="F12" s="42" t="s">
+        <v>427</v>
+      </c>
+      <c r="G12" s="42" t="s">
         <v>400</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="H12" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="42" t="s">
+      <c r="I12" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="J12" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="J12" s="42" t="s">
+      <c r="K12" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="42" t="s">
+      <c r="L12" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="N12" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N12" s="42" t="s">
+      <c r="O12" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O12" s="62" t="s">
+      <c r="P12" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="P12" s="64" t="s">
+      <c r="Q12" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>282</v>
       </c>
-      <c r="Y12" s="42" t="s">
+      <c r="Z12" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB12" s="42" t="s">
+      <c r="AC12" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>283</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>284</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="42">
         <v>12</v>
       </c>
-      <c r="B13" s="46">
-        <v>123456790155</v>
+      <c r="B13" s="11" t="s">
+        <v>413</v>
       </c>
       <c r="C13" s="46">
+        <v>123456790192</v>
+      </c>
+      <c r="D13" s="46">
         <v>123456788</v>
       </c>
-      <c r="D13" s="46">
+      <c r="E13" s="46">
         <v>123456777</v>
       </c>
-      <c r="E13" s="42" t="s">
-        <v>422</v>
-      </c>
       <c r="F13" s="42" t="s">
+        <v>428</v>
+      </c>
+      <c r="G13" s="42" t="s">
         <v>401</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="H13" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="I13" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="J13" s="42" t="s">
         <v>404</v>
       </c>
-      <c r="J13" s="42" t="s">
+      <c r="K13" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="42" t="s">
+      <c r="L13" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="N13" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N13" s="42" t="s">
+      <c r="O13" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="62" t="s">
+      <c r="P13" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="P13" s="65" t="s">
+      <c r="Q13" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="Q13" s="60"/>
-      <c r="W13" t="s">
+      <c r="R13" s="60"/>
+      <c r="X13" t="s">
         <v>282</v>
       </c>
-      <c r="Y13" s="42" t="s">
+      <c r="Z13" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB13" s="42" t="s">
+      <c r="AC13" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>283</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>284</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="42">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C14" s="46">
+        <v>123456790156</v>
+      </c>
+      <c r="D14" s="46">
+        <v>123456788</v>
+      </c>
+      <c r="E14" s="46">
+        <v>123456777</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>414</v>
+      </c>
       <c r="G14" s="42"/>
       <c r="H14" s="42"/>
       <c r="I14" s="42"/>
       <c r="J14" s="42"/>
       <c r="K14" s="42"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="62"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="60"/>
-      <c r="Y14" s="42"/>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" s="42">
-        <v>13</v>
-      </c>
-      <c r="B15" s="46">
+      <c r="L14" s="42"/>
+      <c r="N14" s="43" t="s">
+        <v>407</v>
+      </c>
+      <c r="O14" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q14" s="60" t="s">
+        <v>290</v>
+      </c>
+      <c r="R14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="T14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="U14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="V14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="W14" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="X14" t="s">
+        <v>282</v>
+      </c>
+      <c r="Z14" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>283</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>284</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>285</v>
+      </c>
+      <c r="AH14" s="58" t="s">
+        <v>382</v>
+      </c>
+      <c r="AI14" s="59">
+        <v>1234567898</v>
+      </c>
+      <c r="AJ14" s="58" t="s">
+        <v>383</v>
+      </c>
+      <c r="AK14" s="58" t="s">
+        <v>384</v>
+      </c>
+      <c r="AL14" s="58">
+        <v>84100</v>
+      </c>
+      <c r="AM14" s="58" t="s">
+        <v>385</v>
+      </c>
+      <c r="AN14" s="58" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="42"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="42"/>
+      <c r="Z15" s="42"/>
+      <c r="AH15" s="58"/>
+      <c r="AI15" s="59"/>
+      <c r="AJ15" s="58"/>
+      <c r="AK15" s="58"/>
+      <c r="AL15" s="58"/>
+      <c r="AM15" s="58"/>
+      <c r="AN15" s="58"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" s="42">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="C16" s="46">
         <v>12345679016</v>
       </c>
-      <c r="C15" s="46">
+      <c r="D16" s="46">
         <v>123456788</v>
       </c>
-      <c r="D15" s="46">
+      <c r="E16" s="46">
         <v>123456777</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="F16" s="42" t="s">
         <v>408</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="G16" s="42" t="s">
         <v>402</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="H16" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="42" t="s">
+      <c r="I16" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="J16" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="K16" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="42" t="s">
+      <c r="L16" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="N16" s="43" t="s">
         <v>407</v>
       </c>
-      <c r="N15" s="42" t="s">
+      <c r="O16" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="63" t="s">
+      <c r="P16" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="P15" s="66" t="s">
+      <c r="Q16" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="Q15" s="1"/>
-      <c r="W15" t="s">
+      <c r="R16" s="1"/>
+      <c r="X16" t="s">
         <v>282</v>
       </c>
-      <c r="Y15" s="42" t="s">
+      <c r="Z16" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AB15" s="42" t="s">
+      <c r="AC16" s="42" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="Q16" s="8"/>
-    </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q17" s="8"/>
-    </row>
-    <row r="18" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q18" s="60"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="R17" s="8"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="60"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="AH2" r:id="rId2" display="someone@gmail.com"/>
-    <hyperlink ref="M3:M15" r:id="rId3" display="ab@gmail.com"/>
+    <hyperlink ref="N3:N14" r:id="rId1" display="ab@gmail.com"/>
+    <hyperlink ref="N2" r:id="rId2"/>
+    <hyperlink ref="AI2" r:id="rId3" display="someone@gmail.com"/>
+    <hyperlink ref="N14" r:id="rId4"/>
+    <hyperlink ref="AI14" r:id="rId5" display="someone@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -3612,7 +3784,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,6 +3880,9 @@
       <c r="H3" t="s">
         <v>362</v>
       </c>
+      <c r="I3" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -3779,6 +3954,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>